<commit_message>
Excel file with summary of all the variables
</commit_message>
<xml_diff>
--- a/data_preliminary_analysis.xlsx
+++ b/data_preliminary_analysis.xlsx
@@ -226,10 +226,10 @@
     <t xml:space="preserve">gradeABC</t>
   </si>
   <si>
-    <t xml:space="preserve">Between 0 and 11. Not clear.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48 missings in the original dataset; 39 when merged with oxwaspLbw and 7 when merged also with oxwaspbp</t>
+    <t xml:space="preserve">Between 0 and 11. Sum of how many grades were at least C (&gt;= 5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48 missings in the original dataset; 39 when merged with oxwaspLbw and 7 when merged also with oxwaspbp. Might be useful considering the ratio of A,B,C over the total number of grades obtained.</t>
   </si>
 </sst>
 </file>
@@ -244,6 +244,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -265,6 +266,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -334,7 +336,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,8 +373,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -455,16 +461,16 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="89.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="86.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,7 +749,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,17 +1037,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="7" t="n">
+      <c r="C49" s="9" t="n">
         <v>39</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="10" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
organise data analysis and add imputation script
</commit_message>
<xml_diff>
--- a/data_preliminary_analysis.xlsx
+++ b/data_preliminary_analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SGA Preliminary Analysis" sheetId="1" state="visible" r:id="rId2"/>
@@ -269,7 +269,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +294,12 @@
         <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
@@ -336,7 +342,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -367,6 +373,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -458,19 +468,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="86.1887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="85.1785714285714"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,6 +657,7 @@
       <c r="D15" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
@@ -663,6 +672,7 @@
       <c r="D16" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
@@ -705,6 +715,7 @@
       <c r="D19" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
@@ -750,7 +761,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
@@ -1044,10 +1055,10 @@
       <c r="B49" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="9" t="n">
+      <c r="C49" s="10" t="n">
         <v>39</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="11" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>